<commit_message>
first after 1 official
</commit_message>
<xml_diff>
--- a/data/raw_data_station_801120_fitted.xlsx
+++ b/data/raw_data_station_801120_fitted.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1165" uniqueCount="520">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1143" uniqueCount="509">
   <si>
     <t>evd..fgev</t>
   </si>
@@ -1508,58 +1508,25 @@
     <t xml:space="preserve">[2] "Parameters:"                                                 </t>
   </si>
   <si>
-    <t xml:space="preserve">[3] "      estimate Std. Error"                                   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">[4] "dummy        1         NA"                                   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">[5] "Fixed parameters:"                                           </t>
-  </si>
-  <si>
-    <t xml:space="preserve">[6] "            value"                                           </t>
-  </si>
-  <si>
-    <t xml:space="preserve">[7] "scale    23.39786"                                           </t>
-  </si>
-  <si>
-    <t xml:space="preserve">[8] "location 42.00000"                                           </t>
-  </si>
-  <si>
-    <t xml:space="preserve">[9] "shape     0.00001"                                           </t>
+    <t xml:space="preserve">[3] "Fixed parameters:"                                           </t>
   </si>
   <si>
     <t>$`GoodnessOfFit_fitdistrplus::gofstat`</t>
   </si>
   <si>
-    <t xml:space="preserve"> [1] "Goodness-of-fit statistics"                </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [2] "                             1-mle-mygpd"  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [3] "Kolmogorov-Smirnov statistic   0.0889465"  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [4] "Cramer-von Mises statistic     0.2092053"  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [5] "Anderson-Darling statistic     1.6838894"  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [6] ""                                          </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [7] "Goodness-of-fit criteria"                  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [8] "                               1-mle-mygpd"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [9] "Akaike's Information Criterion    1505.242"</t>
-  </si>
-  <si>
-    <t>[10] "Bayesian Information Criterion    1508.441"</t>
+    <t xml:space="preserve"> [1] "Goodness-of-fit statistics"                 "                             1-mle-mygpd"  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [3] "Kolmogorov-Smirnov statistic   0.0889465"   "Cramer-von Mises statistic     0.2092053"  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [5] "Anderson-Darling statistic     1.6838894"   ""                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [7] "Goodness-of-fit criteria"                   "                               1-mle-mygpd"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [9] "Akaike's Information Criterion    1505.242" "Bayesian Information Criterion    1508.441"</t>
   </si>
   <si>
     <t>$`KolmogorovSmirnovTest_stats::ks.test`</t>
@@ -1729,7 +1696,7 @@
         <v>94</v>
       </c>
       <c r="B6" t="s">
-        <v>496</v>
+        <v>331</v>
       </c>
     </row>
     <row r="7">
@@ -1737,7 +1704,7 @@
         <v>95</v>
       </c>
       <c r="B7" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="8">
@@ -1745,7 +1712,7 @@
         <v>96</v>
       </c>
       <c r="B8" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="9">
@@ -1753,7 +1720,7 @@
         <v>97</v>
       </c>
       <c r="B9" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="10">
@@ -1761,7 +1728,7 @@
         <v>98</v>
       </c>
       <c r="B10" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="11">
@@ -1769,7 +1736,7 @@
         <v>99</v>
       </c>
       <c r="B11" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="12">
@@ -1777,7 +1744,7 @@
         <v>100</v>
       </c>
       <c r="B12" t="s">
-        <v>331</v>
+        <v>501</v>
       </c>
     </row>
     <row r="13">
@@ -1785,7 +1752,7 @@
         <v>101</v>
       </c>
       <c r="B13" t="s">
-        <v>502</v>
+        <v>331</v>
       </c>
     </row>
     <row r="14">
@@ -1793,7 +1760,7 @@
         <v>102</v>
       </c>
       <c r="B14" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="15">
@@ -1801,7 +1768,7 @@
         <v>103</v>
       </c>
       <c r="B15" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="16">
@@ -1809,7 +1776,7 @@
         <v>104</v>
       </c>
       <c r="B16" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="17">
@@ -1817,7 +1784,7 @@
         <v>105</v>
       </c>
       <c r="B17" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="18">
@@ -1825,7 +1792,7 @@
         <v>106</v>
       </c>
       <c r="B18" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="19">
@@ -1833,7 +1800,7 @@
         <v>107</v>
       </c>
       <c r="B19" t="s">
-        <v>508</v>
+        <v>331</v>
       </c>
     </row>
     <row r="20">
@@ -1841,7 +1808,7 @@
         <v>108</v>
       </c>
       <c r="B20" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="21">
@@ -1849,7 +1816,7 @@
         <v>109</v>
       </c>
       <c r="B21" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="22">
@@ -1857,94 +1824,6 @@
         <v>110</v>
       </c>
       <c r="B22" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s">
-        <v>111</v>
-      </c>
-      <c r="B23" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s">
-        <v>112</v>
-      </c>
-      <c r="B24" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="s">
-        <v>113</v>
-      </c>
-      <c r="B25" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="s">
-        <v>114</v>
-      </c>
-      <c r="B26" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="s">
-        <v>115</v>
-      </c>
-      <c r="B27" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="s">
-        <v>116</v>
-      </c>
-      <c r="B28" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="s">
-        <v>117</v>
-      </c>
-      <c r="B29" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="s">
-        <v>118</v>
-      </c>
-      <c r="B30" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="s">
-        <v>119</v>
-      </c>
-      <c r="B31" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="s">
-        <v>120</v>
-      </c>
-      <c r="B32" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="s">
-        <v>121</v>
-      </c>
-      <c r="B33" t="s">
         <v>331</v>
       </c>
     </row>

</xml_diff>

<commit_message>
first after surgery. Fixed graphics por results chapter and size for TIFF images
</commit_message>
<xml_diff>
--- a/data/raw_data_station_801120_fitted.xlsx
+++ b/data/raw_data_station_801120_fitted.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1143" uniqueCount="509">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1165" uniqueCount="520">
   <si>
     <t>evd..fgev</t>
   </si>
@@ -1508,25 +1508,58 @@
     <t xml:space="preserve">[2] "Parameters:"                                                 </t>
   </si>
   <si>
-    <t xml:space="preserve">[3] "Fixed parameters:"                                           </t>
+    <t xml:space="preserve">[3] "      estimate Std. Error"                                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[4] "dummy        1         NA"                                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[5] "Fixed parameters:"                                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[6] "            value"                                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[7] "scale    23.39786"                                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[8] "location 42.00000"                                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[9] "shape     0.00001"                                           </t>
   </si>
   <si>
     <t>$`GoodnessOfFit_fitdistrplus::gofstat`</t>
   </si>
   <si>
-    <t xml:space="preserve"> [1] "Goodness-of-fit statistics"                 "                             1-mle-mygpd"  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [3] "Kolmogorov-Smirnov statistic   0.0889465"   "Cramer-von Mises statistic     0.2092053"  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [5] "Anderson-Darling statistic     1.6838894"   ""                                          </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [7] "Goodness-of-fit criteria"                   "                               1-mle-mygpd"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [9] "Akaike's Information Criterion    1505.242" "Bayesian Information Criterion    1508.441"</t>
+    <t xml:space="preserve"> [1] "Goodness-of-fit statistics"                </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [2] "                             1-mle-mygpd"  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [3] "Kolmogorov-Smirnov statistic   0.0889465"  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [4] "Cramer-von Mises statistic     0.2092053"  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [5] "Anderson-Darling statistic     1.6838894"  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [6] ""                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [7] "Goodness-of-fit criteria"                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [8] "                               1-mle-mygpd"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [9] "Akaike's Information Criterion    1505.242"</t>
+  </si>
+  <si>
+    <t>[10] "Bayesian Information Criterion    1508.441"</t>
   </si>
   <si>
     <t>$`KolmogorovSmirnovTest_stats::ks.test`</t>
@@ -1696,7 +1729,7 @@
         <v>94</v>
       </c>
       <c r="B6" t="s">
-        <v>331</v>
+        <v>496</v>
       </c>
     </row>
     <row r="7">
@@ -1704,7 +1737,7 @@
         <v>95</v>
       </c>
       <c r="B7" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
     </row>
     <row r="8">
@@ -1712,7 +1745,7 @@
         <v>96</v>
       </c>
       <c r="B8" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
     </row>
     <row r="9">
@@ -1720,7 +1753,7 @@
         <v>97</v>
       </c>
       <c r="B9" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
     </row>
     <row r="10">
@@ -1728,7 +1761,7 @@
         <v>98</v>
       </c>
       <c r="B10" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
     </row>
     <row r="11">
@@ -1736,7 +1769,7 @@
         <v>99</v>
       </c>
       <c r="B11" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
     </row>
     <row r="12">
@@ -1744,7 +1777,7 @@
         <v>100</v>
       </c>
       <c r="B12" t="s">
-        <v>501</v>
+        <v>331</v>
       </c>
     </row>
     <row r="13">
@@ -1752,7 +1785,7 @@
         <v>101</v>
       </c>
       <c r="B13" t="s">
-        <v>331</v>
+        <v>502</v>
       </c>
     </row>
     <row r="14">
@@ -1760,7 +1793,7 @@
         <v>102</v>
       </c>
       <c r="B14" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
     <row r="15">
@@ -1768,7 +1801,7 @@
         <v>103</v>
       </c>
       <c r="B15" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
     </row>
     <row r="16">
@@ -1776,7 +1809,7 @@
         <v>104</v>
       </c>
       <c r="B16" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
     </row>
     <row r="17">
@@ -1784,7 +1817,7 @@
         <v>105</v>
       </c>
       <c r="B17" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
     </row>
     <row r="18">
@@ -1792,7 +1825,7 @@
         <v>106</v>
       </c>
       <c r="B18" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
     </row>
     <row r="19">
@@ -1800,7 +1833,7 @@
         <v>107</v>
       </c>
       <c r="B19" t="s">
-        <v>331</v>
+        <v>508</v>
       </c>
     </row>
     <row r="20">
@@ -1808,7 +1841,7 @@
         <v>108</v>
       </c>
       <c r="B20" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
     </row>
     <row r="21">
@@ -1816,7 +1849,7 @@
         <v>109</v>
       </c>
       <c r="B21" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
     </row>
     <row r="22">
@@ -1824,6 +1857,94 @@
         <v>110</v>
       </c>
       <c r="B22" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>111</v>
+      </c>
+      <c r="B23" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>112</v>
+      </c>
+      <c r="B24" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>113</v>
+      </c>
+      <c r="B25" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>114</v>
+      </c>
+      <c r="B26" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>115</v>
+      </c>
+      <c r="B27" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>116</v>
+      </c>
+      <c r="B28" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>117</v>
+      </c>
+      <c r="B29" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>118</v>
+      </c>
+      <c r="B30" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>119</v>
+      </c>
+      <c r="B31" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>120</v>
+      </c>
+      <c r="B32" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>121</v>
+      </c>
+      <c r="B33" t="s">
         <v>331</v>
       </c>
     </row>

</xml_diff>